<commit_message>
revise Midterm One weights
</commit_message>
<xml_diff>
--- a/course_materials/Intro_Bayes_Course_course_assessment_plan.xlsx
+++ b/course_materials/Intro_Bayes_Course_course_assessment_plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfred/OneDrive - University of Nevada, Reno/Teaching/Bayes_course/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfred/OneDrive - University of Nevada, Reno/Teaching/Bayes_course/git_public/course_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB7A44B-418C-4B40-954A-EED419F8E334}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C28145B-3DC6-6F4D-B960-8CE1A491492A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28240" xr2:uid="{817317F3-93E4-1348-8419-7945FAAB9BF9}"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{817317F3-93E4-1348-8419-7945FAAB9BF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,10 +886,10 @@
         <v>10</v>
       </c>
       <c r="C17">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
@@ -1055,11 +1055,11 @@
       </c>
       <c r="C23" s="1">
         <f t="shared" ref="C23:I23" si="1">SUM(C2:C22)</f>
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="1"/>
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="1"/>
@@ -1096,11 +1096,11 @@
       </c>
       <c r="C24" s="1">
         <f>(C23/I23)*100</f>
-        <v>16.25</v>
+        <v>18.125</v>
       </c>
       <c r="D24" s="1">
         <f>(D23/I23)*100</f>
-        <v>25.624999999999996</v>
+        <v>23.75</v>
       </c>
       <c r="E24" s="1">
         <f>(E23/I23)*100</f>
@@ -1133,11 +1133,11 @@
       </c>
       <c r="C25" s="1">
         <f>(C23/(I23-I22))*100</f>
-        <v>20</v>
+        <v>22.30769230769231</v>
       </c>
       <c r="D25" s="1">
         <f>(D23/(I23-I22))*100</f>
-        <v>31.538461538461537</v>
+        <v>29.230769230769234</v>
       </c>
       <c r="E25" s="1">
         <f>(E23/(I23-I22))*100</f>

</xml_diff>

<commit_message>
update course materials after midterm two
</commit_message>
<xml_diff>
--- a/course_materials/Intro_Bayes_Course_course_assessment_plan.xlsx
+++ b/course_materials/Intro_Bayes_Course_course_assessment_plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfred/OneDrive - University of Nevada, Reno/Teaching/Bayes_course/git_public/course_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C28145B-3DC6-6F4D-B960-8CE1A491492A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76A9943-09E9-074A-A022-DF559F8A8CBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{817317F3-93E4-1348-8419-7945FAAB9BF9}"/>
+    <workbookView xWindow="-5800" yWindow="4220" windowWidth="33600" windowHeight="20540" xr2:uid="{817317F3-93E4-1348-8419-7945FAAB9BF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,13 +909,13 @@
         <v>14</v>
       </c>
       <c r="C18">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D18">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G18">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
@@ -1055,11 +1055,11 @@
       </c>
       <c r="C23" s="1">
         <f t="shared" ref="C23:I23" si="1">SUM(C2:C22)</f>
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="1"/>
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="1"/>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="G23" s="1">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="1"/>
@@ -1096,11 +1096,11 @@
       </c>
       <c r="C24" s="1">
         <f>(C23/I23)*100</f>
-        <v>18.125</v>
+        <v>16</v>
       </c>
       <c r="D24" s="1">
         <f>(D23/I23)*100</f>
-        <v>23.75</v>
+        <v>24</v>
       </c>
       <c r="E24" s="1">
         <f>(E23/I23)*100</f>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="G24" s="1">
         <f>(G23/I23)*100</f>
-        <v>8.75</v>
+        <v>10.625</v>
       </c>
       <c r="H24" s="1">
         <f>(H23/I23)*100</f>
@@ -1133,11 +1133,11 @@
       </c>
       <c r="C25" s="1">
         <f>(C23/(I23-I22))*100</f>
-        <v>22.30769230769231</v>
+        <v>19.692307692307693</v>
       </c>
       <c r="D25" s="1">
         <f>(D23/(I23-I22))*100</f>
-        <v>29.230769230769234</v>
+        <v>29.53846153846154</v>
       </c>
       <c r="E25" s="1">
         <f>(E23/(I23-I22))*100</f>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="G25" s="1">
         <f>(G23/(I23-I22))*100</f>
-        <v>10.76923076923077</v>
+        <v>13.076923076923078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>